<commit_message>
Site updated: 2019-10-01 16:01:13
</commit_message>
<xml_diff>
--- a/medias/assets/data/data.xlsx
+++ b/medias/assets/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuoranliu/ZL_Asica/Websites/aifans_cc/blog/themes/matery/source/medias/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251B5163-55FE-EB4B-80C9-085293CB3B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15E889A-BAA4-8D45-A5ED-D0E19339CA84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>wechat</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -215,6 +215,10 @@
   </si>
   <si>
     <t>*卜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器首月</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1104,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DCC84F-7839-468C-8148-23D61A6A007E}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1138,10 +1142,10 @@
         <v>36</v>
       </c>
       <c r="C2" s="2">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1149,75 +1153,85 @@
         <v>20190812</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>20190827</v>
+        <v>20190812</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>20190830</v>
+        <v>20190827</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2">
         <v>36</v>
       </c>
-      <c r="C5" s="2">
-        <v>29</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>20190826</v>
+        <v>20190830</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
+        <v>20190826</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
         <v>20190912</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>80.099999999999994</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4"/>
-    <row r="9" spans="1:4"/>
-    <row r="10" spans="1:4"/>
-    <row r="11" spans="1:4"/>
     <row r="12" spans="1:4">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
@@ -1612,11 +1626,11 @@
       </c>
       <c r="H9">
         <f>SUMIFS(out!C:C,out!A:A,"&gt;20190800",out!A:A,"&lt;20190900")</f>
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>640.66</v>
+        <v>560.66</v>
       </c>
     </row>
     <row r="10" spans="1:9">

</xml_diff>

<commit_message>
Site updated: 2019-10-07 19:52:39
</commit_message>
<xml_diff>
--- a/medias/assets/data/data.xlsx
+++ b/medias/assets/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuoranliu/ZL_Asica/Websites/aifans_cc/blog/themes/matery/source/medias/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15E889A-BAA4-8D45-A5ED-D0E19339CA84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAB4292-8BF7-E846-AE89-F49D5785968E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>wechat</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -218,7 +218,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>服务器首月</t>
+    <t>服务器首周</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>半月服务器费用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAKED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keishi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B站年度大会员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*翔辰</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -555,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -897,7 +921,7 @@
         <v>32</v>
       </c>
       <c r="C24" s="1">
-        <v>171.15</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>0</v>
@@ -918,22 +942,46 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1">
+        <v>20191005</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="A27" s="1">
+        <v>20191007</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1">
+        <v>100</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="A28" s="1">
+        <v>20191007</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1"/>
@@ -1106,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DCC84F-7839-468C-8148-23D61A6A007E}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1220,22 +1268,45 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
+        <v>20190901</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2">
         <v>20190912</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>80.099999999999994</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2">
+        <v>20191003</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2">
+        <v>98</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3"/>
@@ -1291,6 +1362,11 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1639,7 +1715,7 @@
       </c>
       <c r="B10">
         <f>SUMIFS(in!C:C,in!A:A,"&gt;20190900",in!A:A,"&lt;20191000")</f>
-        <v>993.15</v>
+        <v>883</v>
       </c>
       <c r="C10">
         <f>SUMIFS(in!C:C,in!D:D,"=alipay",in!A:A,"&gt;20190900",in!A:A,"&lt;20191000")</f>
@@ -1647,7 +1723,7 @@
       </c>
       <c r="D10">
         <f>SUMIFS(in!C:C,in!D:D,"=wechat",in!A:A,"&gt;20190900",in!A:A,"&lt;20191000")</f>
-        <v>174.15</v>
+        <v>64</v>
       </c>
       <c r="E10">
         <f>SUMIFS(in!C:C,in!D:D,"=bilibili",in!A:A,"&gt;20190900",in!A:A,"&lt;20191000")</f>
@@ -1663,11 +1739,11 @@
       </c>
       <c r="H10">
         <f>SUMIFS(out!C:C,out!A:A,"&gt;20190900",out!A:A,"&lt;20191000")</f>
-        <v>80.099999999999994</v>
+        <v>121.1</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>913.05</v>
+        <v>761.9</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1676,15 +1752,15 @@
       </c>
       <c r="B11">
         <f>SUMIFS(in!C:C,in!A:A,"&gt;20191000",in!A:A,"&lt;20191100")</f>
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="C11">
         <f>SUMIFS(in!C:C,in!D:D,"=alipay",in!A:A,"&gt;20191000",in!A:A,"&lt;20191100")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <f>SUMIFS(in!C:C,in!D:D,"=wechat",in!A:A,"&gt;20191000",in!A:A,"&lt;20191100")</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="E11">
         <f>SUMIFS(in!C:C,in!D:D,"=bilibili",in!A:A,"&gt;20191000",in!A:A,"&lt;20191100")</f>
@@ -1700,11 +1776,11 @@
       </c>
       <c r="H11">
         <f>SUMIFS(out!C:C,out!A:A,"&gt;20191000",out!A:A,"&lt;20191100")</f>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9">

</xml_diff>

<commit_message>
Site updated: 2019-10-15 20:07:57
</commit_message>
<xml_diff>
--- a/medias/assets/data/data.xlsx
+++ b/medias/assets/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuoranliu/ZL_Asica/Websites/aifans_cc/blog/themes/matery/source/medias/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAB4292-8BF7-E846-AE89-F49D5785968E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EF257A-BD62-4740-855B-18B09734E518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4540" windowWidth="18340" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>wechat</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,6 +243,10 @@
   </si>
   <si>
     <t>*翔辰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器10月费用</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -579,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="150" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -1156,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DCC84F-7839-468C-8148-23D61A6A007E}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1306,6 +1310,20 @@
       </c>
       <c r="D10" s="2" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>20191010</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2">
+        <v>80.2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1776,11 +1794,11 @@
       </c>
       <c r="H11">
         <f>SUMIFS(out!C:C,out!A:A,"&gt;20191000",out!A:A,"&lt;20191100")</f>
-        <v>98</v>
+        <v>178.2</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>-70.199999999999989</v>
       </c>
     </row>
     <row r="12" spans="1:9">

</xml_diff>